<commit_message>
Changes: - Changed: Minor changes of the default config files BugFix: - Fixed: rank score error when no peak identified - Fixed: FA whitelist header now auto convert to all CAPITAL in Hunter - Fixed: Change Lipid_type to lipid_class - Fixed: Isotope score specific bug in Thermo files
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/1-FA_Whitelist_PL.xlsx
+++ b/ConfigurationFiles/1-FA_Whitelist_PL.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{39A848DD-FC7E-4473-ADDE-692410873F36}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="27">
   <si>
     <t>FattyAcid</t>
   </si>
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,18 +116,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,7 +138,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,19 +418,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +453,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -471,11 +466,14 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
       <c r="G2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -495,7 +493,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -508,11 +506,14 @@
       <c r="D4" t="s">
         <v>18</v>
       </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -532,7 +533,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -552,7 +553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -572,10 +573,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
@@ -589,10 +593,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
@@ -606,10 +613,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
@@ -623,10 +633,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
@@ -640,10 +653,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
@@ -657,10 +673,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
@@ -674,10 +693,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
@@ -691,7 +713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -702,7 +724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -713,7 +735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -724,7 +746,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -735,7 +757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -746,7 +768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>

</xml_diff>